<commit_message>
changed the order of atd class in rats subgroups plot
</commit_message>
<xml_diff>
--- a/data/subgruposppt.xlsx
+++ b/data/subgruposppt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/tamires_martins_ufsc_br/Documents/PROJETO_R_GITHUB/sbfte_martins2023_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{C1C7C836-8328-450F-9C24-F0B29ADFBD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38F46A03-DF3A-4D84-9F1D-99DA94899157}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{C1C7C836-8328-450F-9C24-F0B29ADFBD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3051EA88-03AD-470A-B8BE-176EAABDCF68}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -819,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="K95" sqref="K95"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3961,31 +3961,31 @@
         <v>54</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="E90" s="9">
-        <v>0.73</v>
+        <v>2.52</v>
       </c>
       <c r="F90" s="9">
-        <v>-0.3</v>
+        <v>0.63</v>
       </c>
       <c r="G90" s="9">
-        <v>1.76</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="H90" s="9">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I90" s="9">
-        <v>79.069999999999993</v>
+        <v>72.930000000000007</v>
       </c>
       <c r="J90" s="9" t="s">
         <v>75</v>
       </c>
       <c r="K90" s="1">
-        <v>1.92</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -3999,28 +3999,28 @@
         <v>65</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="E91" s="9">
-        <v>1.35</v>
+        <v>0.73</v>
       </c>
       <c r="F91" s="9">
-        <v>-0.1</v>
+        <v>-0.3</v>
       </c>
       <c r="G91" s="9">
-        <v>2.79</v>
+        <v>1.76</v>
       </c>
       <c r="H91" s="9">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I91" s="9">
-        <v>82.54</v>
+        <v>79.069999999999993</v>
       </c>
       <c r="J91" s="9" t="s">
         <v>75</v>
       </c>
       <c r="K91" s="1">
-        <v>2.64</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
@@ -4034,28 +4034,28 @@
         <v>65</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E92" s="9">
-        <v>-0.36</v>
+        <v>1.35</v>
       </c>
       <c r="F92" s="9">
-        <v>-1.1000000000000001</v>
+        <v>-0.1</v>
       </c>
       <c r="G92" s="9">
-        <v>0.39</v>
+        <v>2.79</v>
       </c>
       <c r="H92" s="9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I92" s="9">
-        <v>0</v>
+        <v>82.54</v>
       </c>
       <c r="J92" s="9" t="s">
         <v>75</v>
       </c>
       <c r="K92" s="1">
-        <v>0</v>
+        <v>2.64</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -4066,31 +4066,31 @@
         <v>54</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="E93" s="9">
-        <v>2.52</v>
+        <v>-0.36</v>
       </c>
       <c r="F93" s="9">
-        <v>0.63</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="G93" s="9">
-        <v>4.4000000000000004</v>
+        <v>0.39</v>
       </c>
       <c r="H93" s="9">
         <v>3</v>
       </c>
       <c r="I93" s="9">
-        <v>72.930000000000007</v>
+        <v>0</v>
       </c>
       <c r="J93" s="9" t="s">
         <v>75</v>
       </c>
       <c r="K93" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>